<commit_message>
Two records added to excelsheet
</commit_message>
<xml_diff>
--- a/ExcelSheet.xlsx
+++ b/ExcelSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>S No</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>resrewr</t>
+  </si>
+  <si>
+    <t>qdasdsd</t>
   </si>
 </sst>
 </file>
@@ -356,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,6 +385,28 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>